<commit_message>
work diary minimum upgrades
</commit_message>
<xml_diff>
--- a/LIBELLULA(diario).xlsx
+++ b/LIBELLULA(diario).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\OneDrive\Desktop\Libellula\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0037e56ddff3a368/Desktop/Libellula/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A320F2B-9005-4399-9E48-5F210EFD5E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{1A320F2B-9005-4399-9E48-5F210EFD5E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAA68E89-DB5C-4F7B-95A0-CA494E025B19}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CC99F97F-3E72-4FEA-AA64-B39819E65309}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>PLANEJAMENTO LIBELLULA (secreto)</t>
   </si>
@@ -84,22 +84,38 @@
   </si>
   <si>
     <t>00h00-01h38</t>
+  </si>
+  <si>
+    <t>Quinta-feira, 12/02/26</t>
+  </si>
+  <si>
+    <t>23h00-00h30</t>
+  </si>
+  <si>
+    <t>1) Ferramentas financeiras criadas e repositório atualizado com a inclusão das mesmas.</t>
+  </si>
+  <si>
+    <t>1) Codei diversas ferramentas e indicadores, desde médias móveis básicas até ociladores estocásticos, tudo já atualizado no repositório remoto.</t>
+  </si>
+  <si>
+    <t>Usei o livro "Machine Learning &amp; Data Science Blueprints for Finance", de Hariom Tatsat, Sahil Puri and Brad Lookabaugh, p. 181-184</t>
+  </si>
+  <si>
+    <t>Sem alterações</t>
+  </si>
+  <si>
+    <t>Sem atualizações de estrutura</t>
+  </si>
+  <si>
+    <t>Sem bugs relatados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -186,17 +202,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -213,6 +228,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,17 +586,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A98371-216A-4D1C-8D7B-786B21A1BFEF}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" style="13" customWidth="1"/>
+    <col min="1" max="2" width="12.7109375" style="12" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="9" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" style="5" customWidth="1"/>
     <col min="7" max="7" width="30.7109375" style="7" customWidth="1"/>
@@ -605,10 +638,10 @@
       <c r="H3"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -631,21 +664,55 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="15" t="s">
+      <c r="D5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="F5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="15" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>